<commit_message>
Validar programa de pagos en BC
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Validar Programa de Pagos.xlsx
+++ b/Sura/DataSource - Validar Programa de Pagos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7295904D-1388-43B8-BBD6-1B18E0A58F25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8199DE-F77A-4461-93F8-301E51296EB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{57A6CF53-9997-4B4E-BF87-51EB0D7B0BBF}"/>
   </bookViews>
@@ -48,29 +48,37 @@
     <t>gw</t>
   </si>
   <si>
+    <t>suragwqa2.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>12112002274</t>
+  </si>
+  <si>
+    <t>12112002275</t>
+  </si>
+  <si>
+    <t>12112002276</t>
+  </si>
+  <si>
     <t>https://suragwqa2.segurossura.com.ar/pc/PolicyCenter.do</t>
-  </si>
-  <si>
-    <t>suragwqa2.segurossura.com.ar</t>
-  </si>
-  <si>
-    <t>12112002274</t>
-  </si>
-  <si>
-    <t>12112002275</t>
-  </si>
-  <si>
-    <t>12112002276</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,14 +101,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,10 +427,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -440,10 +454,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
         <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -451,16 +465,16 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -468,16 +482,16 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
         <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -485,8 +499,8 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>